<commit_message>
Combined Sorghum_BW8 simulations into a single experiment.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -232,40 +232,40 @@
     <t xml:space="preserve">IcrisatBW5CvQL41xQL36FertLowIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T2</t>
+    <t xml:space="preserve">IcrisatBW8CvCSH13RFertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T1</t>
+    <t xml:space="preserve">IcrisatBW8CvM35-1FertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T3</t>
+    <t xml:space="preserve">IcrisatBW8CvAtx623xRTx430FertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T4</t>
+    <t xml:space="preserve">IcrisatBW8CvQL41xQL36FertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T5</t>
+    <t xml:space="preserve">IcrisatBW8CvM35-1FertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T6</t>
+    <t xml:space="preserve">IcrisatBW8CvCSH13RFertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T7</t>
+    <t xml:space="preserve">IcrisatBW8CvATX623xRTX430FertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T8</t>
+    <t xml:space="preserve">IcrisatBW8CvQL41xQL36FertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T9</t>
+    <t xml:space="preserve">IcrisatBW8CvM35-1FertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T10</t>
+    <t xml:space="preserve">IcrisatBW8CvCSH13RFertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T11</t>
+    <t xml:space="preserve">IcrisatBW8CvATX623xRTX430FertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_BW8_GxE_T12</t>
+    <t xml:space="preserve">IcrisatBW8CvQL41xQL36FertLowIrrigOff</t>
   </si>
   <si>
     <t xml:space="preserve">Hermitage1996FertHighIrrigOnCvBuster</t>
@@ -608,10 +608,10 @@
   <dimension ref="A1:BE2195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="26" sqref="B10 B28 B46 B57 B69 B77 B87 B99 B107 B119 B140 B148 B152 B154 B163 B175 B187 B195 B205 B217 B231 B242 B260 B270 B277 B293 I14"/>
+      <selection pane="topLeft" activeCell="L14" activeCellId="28" sqref="B307 B330 B338 B352 B356 B366 B378 B386 B396 B408 B416 B426 B441 B449 B454 B465 B477 B489 B496 B506 B518 B526 B540 B546 B557 B560 B573 B592 L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.86"/>

</xml_diff>

<commit_message>
Combined sorghum LE14 simulations into a single experiment.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -358,13 +358,13 @@
     <t xml:space="preserve">Sorghum_LE13_M35-1+I+N</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE14_Buster</t>
+    <t xml:space="preserve">Lawes1996EarlyCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE14_QL41xQL36</t>
+    <t xml:space="preserve">Lawes1996EarlyCvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE14_M35-1</t>
+    <t xml:space="preserve">Lawes1996EarlyCvM351-1</t>
   </si>
   <si>
     <t xml:space="preserve">Sorghum_LE15_Buster</t>
@@ -608,7 +608,7 @@
   <dimension ref="A1:BE2195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="28" sqref="B307 B330 B338 B352 B356 B366 B378 B386 B396 B408 B416 B426 B441 B449 B454 B465 B477 B489 B496 B506 B518 B526 B540 B546 B557 B560 B573 B592 L14"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Convert Sorghum_LE13_* simulations into an experiment.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -340,22 +340,22 @@
     <t xml:space="preserve">Hermitage1997FertLowIrrigLowCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE13_Buster-I-N</t>
+    <t xml:space="preserve">Lawes1995FertLowirrigOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE13_Buster-I+N</t>
+    <t xml:space="preserve">Lawes1995FertHighIrrigOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE13_Buster+I+N</t>
+    <t xml:space="preserve">Lawes1995FertHighIrrigOnCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE13_M35-1-I-N</t>
+    <t xml:space="preserve">Lawes1995FertLowIrrigOffCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE13_M35-1-I+N</t>
+    <t xml:space="preserve">Lawes1995FertHighIrrigOffCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE13_M35-1+I+N</t>
+    <t xml:space="preserve">Lawes1995FertHighIrrigOnCvM351</t>
   </si>
   <si>
     <t xml:space="preserve">Lawes1996EarlyCvBuster</t>
@@ -608,7 +608,7 @@
   <dimension ref="A1:BE2195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="L16" activeCellId="22" sqref="B1354 B1360 B1366 B1375 B1381 B1387 B1394 B1400 B1406 B1416 B1419 B1421 B1427:B1428 B1436 B1444 B1450 B1460 B1468 B1470 B1472:B1473 B1476 B1478 L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Convert Sorghum_LE15_* simulations into an experiment.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -367,13 +367,13 @@
     <t xml:space="preserve">Lawes1996EarlyCvM351-1</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE15_Buster</t>
+    <t xml:space="preserve">Lawes1996LateCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE15_QL41xQL36</t>
+    <t xml:space="preserve">Lawes1996LateCvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE15_M35-1</t>
+    <t xml:space="preserve">Lawes1996LateCvM351</t>
   </si>
   <si>
     <t xml:space="preserve">Sorghum_LE17_T1</t>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:BE2195"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="22" sqref="B1354 B1360 B1366 B1375 B1381 B1387 B1394 B1400 B1406 B1416 B1419 B1421 B1427:B1428 B1436 B1444 B1450 B1460 B1468 B1470 B1472:B1473 B1476 B1478 L16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I110" activeCellId="0" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Convert Sorghum_LE17_* simulations into an experiment.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -376,13 +376,13 @@
     <t xml:space="preserve">Lawes1996LateCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE17_T1</t>
+    <t xml:space="preserve">Lawes1997LateCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE17_T3</t>
+    <t xml:space="preserve">Lawes1997LateCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE17_T2</t>
+    <t xml:space="preserve">Lawes1997LateCvM351</t>
   </si>
   <si>
     <t xml:space="preserve">Sorghum_LE19_T3</t>
@@ -608,7 +608,7 @@
   <dimension ref="A1:BE2195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I110" activeCellId="0" sqref="I110"/>
+      <selection pane="topLeft" activeCell="M96" activeCellId="20" sqref="B1638 B1640 B1643 B1646 B1648:B1649 B1652 B1655 B1658 B1661 B1664 B1667 B1671:B1672 B1675 B1678 B1683 B1686 B1689 B1692 B1695:B1696 B1699 M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Convert Sorghum_LE19_* simulations into an experiment.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -385,28 +385,28 @@
     <t xml:space="preserve">Lawes1997LateCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T3</t>
+    <t xml:space="preserve">Lawes1998FertMedBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T6</t>
+    <t xml:space="preserve">Lawes1998FertLowCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T1</t>
+    <t xml:space="preserve">Lawes1998FertOffBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T2</t>
+    <t xml:space="preserve">Lawes1998FertLowBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T4</t>
+    <t xml:space="preserve">Lawes1998FertHighBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T5</t>
+    <t xml:space="preserve">Lawes1998FertOffCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T7</t>
+    <t xml:space="preserve">Lawes1998FertMedCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_LE19_T8</t>
+    <t xml:space="preserve">Lawes1998FertHighCSH13R</t>
   </si>
   <si>
     <t xml:space="preserve">Sorghum_Gatton_RUE_2</t>
@@ -608,7 +608,7 @@
   <dimension ref="A1:BE2195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M96" activeCellId="20" sqref="B1638 B1640 B1643 B1646 B1648:B1649 B1652 B1655 B1658 B1661 B1664 B1667 B1671:B1672 B1675 B1678 B1683 B1686 B1689 B1692 B1695:B1696 B1699 M96"/>
+      <selection pane="topLeft" activeCell="I99" activeCellId="0" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Convert Sorghum_LE21_* simulations into an experiment.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -409,31 +409,31 @@
     <t xml:space="preserve">Lawes1998FertHighCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_2</t>
+    <t xml:space="preserve">Lawes1999FertLowCvA35xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_8</t>
+    <t xml:space="preserve">Lawes1999FertHighCvA35xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_1</t>
+    <t xml:space="preserve">Lawes1999FertLowCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_3</t>
+    <t xml:space="preserve">Lawes1999FertLowCvQL39xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_4</t>
+    <t xml:space="preserve">Lawes1999FertMedCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_5</t>
+    <t xml:space="preserve">Lawes1999FertMedCvA35xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_6</t>
+    <t xml:space="preserve">Lawes1999FertMedCvQL39xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_9</t>
+    <t xml:space="preserve">Lawes1999FertHighCvQL39xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorghum_Gatton_RUE_7</t>
+    <t xml:space="preserve">Lawes1999FertHighCvCSH13R</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:BE2195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I99" activeCellId="0" sqref="I99"/>
+      <selection pane="topLeft" activeCell="O98" activeCellId="32" sqref="B1899 B1910 B1919 B1928 B1935 B1939 B1941 B1950 B1959 B1973 B1982 B1991 B1993 B1997 B2007 B2021 B2031 B2035 B2038 B2050 B2065 B2078 B2095 B2105 B2114 B2123 B2132 B2141 B2143 B2152 B2154 B2171 O98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed some typos in simulation name mappings in sorghum observed data.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -364,7 +364,7 @@
     <t xml:space="preserve">Lawes1996EarlyCvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1996EarlyCvM351-1</t>
+    <t xml:space="preserve">Lawes1996EarlyCvM351</t>
   </si>
   <si>
     <t xml:space="preserve">Lawes1996LateCvBuster</t>
@@ -385,55 +385,55 @@
     <t xml:space="preserve">Lawes1997LateCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertMedBuster</t>
+    <t xml:space="preserve">Lawes1998FertMedCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertLowCSH13R</t>
+    <t xml:space="preserve">Lawes1998FertLowCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertOffBuster</t>
+    <t xml:space="preserve">Lawes1998FertOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertLowBuster</t>
+    <t xml:space="preserve">Lawes1998FertLowCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertHighBuster</t>
+    <t xml:space="preserve">Lawes1998FertHighCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertOffCSH13R</t>
+    <t xml:space="preserve">Lawes1998FertOffCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertMedCSH13R</t>
+    <t xml:space="preserve">Lawes1998FertMedCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertHighCSH13R</t>
+    <t xml:space="preserve">Lawes1998FertHighCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertLowCvA35xQL36</t>
+    <t xml:space="preserve">Lawes1999CvA35xQL36FertLow</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertHighCvA35xQL36</t>
+    <t xml:space="preserve">Lawes1999CvA35xQL36FertHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertLowCvCSH13R</t>
+    <t xml:space="preserve">Lawes1999CvCSH13RFertLow</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertLowCvQL39xQL36</t>
+    <t xml:space="preserve">Lawes1999CvQL39xQL36FertLow</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertMedCvCSH13R</t>
+    <t xml:space="preserve">Lawes1999CvCSH13RFertMed</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertMedCvA35xQL36</t>
+    <t xml:space="preserve">Lawes1999CvA35xQL36FertMed</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertMedCvQL39xQL36</t>
+    <t xml:space="preserve">Lawes1999CvQL39xQL36FertMed</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertHighCvQL39xQL36</t>
+    <t xml:space="preserve">Lawes1999CvQL39xQL36FertHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999FertHighCvCSH13R</t>
+    <t xml:space="preserve">Lawes1999CvCSH13RFertHigh</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:BE2195"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O98" activeCellId="32" sqref="B1899 B1910 B1919 B1928 B1935 B1939 B1941 B1950 B1959 B1973 B1982 B1991 B1993 B1997 B2007 B2021 B2031 B2035 B2038 B2050 B2065 B2078 B2095 B2105 B2114 B2123 B2132 B2141 B2143 B2152 B2154 B2171 O98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1812" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1820" activeCellId="32" sqref="B1899 B1910 B1919 B1928 B1935 B1939 B1941 B1950 B1959 B1973 B1982 B1991 B1993 B1997 B2007 B2021 B2031 B2035 B2038 B2050 B2065 B2078 B2095 B2105 B2114 B2123 B2132 B2141 B2143 B2152 B2154 B2171 C1820"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update sorghum experiment names.
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -196,244 +196,244 @@
     <t xml:space="preserve">TPLA</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvM35-1FertHighIrrigHigh</t>
+    <t xml:space="preserve">BW5CvM35-1FertHighIrrigHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvCSH13RFertHighIrrigHigh</t>
+    <t xml:space="preserve">BW5CvCSH13RFertHighIrrigHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvAtx623xRTX430FertHighIrrigHigh</t>
+    <t xml:space="preserve">BW5CvAtx623xRTX430FertHighIrrigHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvQL41xQL36FertHighIrrigHigh</t>
+    <t xml:space="preserve">BW5CvQL41xQL36FertHighIrrigHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvM35-1FertMedIrrigLow</t>
+    <t xml:space="preserve">BW5CvM35-1FertMedIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvCSH13RFertMedIrrigLow</t>
+    <t xml:space="preserve">BW5CvCSH13RFertMedIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvAtx623xRTX430FertMedIrrigLow</t>
+    <t xml:space="preserve">BW5CvAtx623xRTX430FertMedIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvQL41xQL36FertMedIrrigLow</t>
+    <t xml:space="preserve">BW5CvQL41xQL36FertMedIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvM35-1FertLowIrrigLow</t>
+    <t xml:space="preserve">BW5CvM35-1FertLowIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvCSH13RFertLowIrrigLow</t>
+    <t xml:space="preserve">BW5CvCSH13RFertLowIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvAtx623xRTX430FertLowIrrigLow</t>
+    <t xml:space="preserve">BW5CvAtx623xRTX430FertLowIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW5CvQL41xQL36FertLowIrrigLow</t>
+    <t xml:space="preserve">BW5CvQL41xQL36FertLowIrrigLow</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvCSH13RFertHighIrrigOn</t>
+    <t xml:space="preserve">BW8CvCSH13RFertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvM35-1FertHighIrrigOn</t>
+    <t xml:space="preserve">BW8CvM35-1FertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvAtx623xRTx430FertHighIrrigOn</t>
+    <t xml:space="preserve">BW8CvAtx623xRTx430FertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvQL41xQL36FertHighIrrigOn</t>
+    <t xml:space="preserve">BW8CvQL41xQL36FertHighIrrigOn</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvM35-1FertMedIrrigOff</t>
+    <t xml:space="preserve">BW8CvM35-1FertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvCSH13RFertMedIrrigOff</t>
+    <t xml:space="preserve">BW8CvCSH13RFertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvATX623xRTX430FertMedIrrigOff</t>
+    <t xml:space="preserve">BW8CvATX623xRTX430FertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvQL41xQL36FertMedIrrigOff</t>
+    <t xml:space="preserve">BW8CvQL41xQL36FertMedIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvM35-1FertLowIrrigOff</t>
+    <t xml:space="preserve">BW8CvM35-1FertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvCSH13RFertLowIrrigOff</t>
+    <t xml:space="preserve">BW8CvCSH13RFertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvATX623xRTX430FertLowIrrigOff</t>
+    <t xml:space="preserve">BW8CvATX623xRTX430FertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">IcrisatBW8CvQL41xQL36FertLowIrrigOff</t>
+    <t xml:space="preserve">BW8CvQL41xQL36FertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertHighIrrigOnCvBuster</t>
+    <t xml:space="preserve">HE1-4FertHighIrrigOnCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertHighIrrigOnCvQL41xQL36</t>
+    <t xml:space="preserve">HE1-4FertHighIrrigOnCvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertHighIrrigOnCvM351</t>
+    <t xml:space="preserve">HE1-4FertHighIrrigOnCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertLowIrrigOnCvQL41xQL36</t>
+    <t xml:space="preserve">HE1-4FertLowIrrigOnCvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertLowIrrigOnCvBuster</t>
+    <t xml:space="preserve">HE1-4FertLowIrrigOnCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertLowIrrigOnCvM351</t>
+    <t xml:space="preserve">HE1-4FertLowIrrigOnCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertHighIrrigOffCvQL41xQL36</t>
+    <t xml:space="preserve">HE1-4FertHighIrrigOffCvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertHighIrrigOffCvBuster</t>
+    <t xml:space="preserve">HE1-4FertHighIrrigOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertHighIrrigOffCvM351</t>
+    <t xml:space="preserve">HE1-4FertHighIrrigOffCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertLowIrrigOffCvQL41xQL36</t>
+    <t xml:space="preserve">HE1-4FertLowIrrigOffCvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertLowIrrigOffCvBuster</t>
+    <t xml:space="preserve">HE1-4FertLowIrrigOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1996FertLowIrrigOffCvM351</t>
+    <t xml:space="preserve">HE1-4FertLowIrrigOffCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertHighIrrigHighCvBuster</t>
+    <t xml:space="preserve">HE5-8FertHighIrrigHighCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertHighIrrigHighCvM351</t>
+    <t xml:space="preserve">HE5-8FertHighIrrigHighCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertHighIrrigHighCvCSH13R</t>
+    <t xml:space="preserve">HE5-8FertHighIrrigHighCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertLowIrrigHighCvBuster</t>
+    <t xml:space="preserve">HE5-8FertLowIrrigHighCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertLowIrrigHighCvM351</t>
+    <t xml:space="preserve">HE5-8FertLowIrrigHighCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertLowIrrigHighCvCSH13R</t>
+    <t xml:space="preserve">HE5-8FertLowIrrigHighCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertHighIrrigLowCvBuster</t>
+    <t xml:space="preserve">HE5-8FertHighIrrigLowCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertHighIrrigLowCvM351</t>
+    <t xml:space="preserve">HE5-8FertHighIrrigLowCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertHighIrrigLowCvCSH13R</t>
+    <t xml:space="preserve">HE5-8FertHighIrrigLowCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertLowIrrigLowCvBuster</t>
+    <t xml:space="preserve">HE5-8FertLowIrrigLowCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertLowIrrigLowCvM351</t>
+    <t xml:space="preserve">HE5-8FertLowIrrigLowCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Hermitage1997FertLowIrrigLowCvCSH13R</t>
+    <t xml:space="preserve">HE5-8FertLowIrrigLowCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1995FertLowirrigOffCvBuster</t>
+    <t xml:space="preserve">LE13FertLowirrigOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1995FertHighIrrigOffCvBuster</t>
+    <t xml:space="preserve">LE13FertHighIrrigOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1995FertHighIrrigOnCvBuster</t>
+    <t xml:space="preserve">LE13FertHighIrrigOnCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1995FertLowIrrigOffCvM351</t>
+    <t xml:space="preserve">LE13FertLowIrrigOffCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1995FertHighIrrigOffCvM351</t>
+    <t xml:space="preserve">LE13FertHighIrrigOffCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1995FertHighIrrigOnCvM351</t>
+    <t xml:space="preserve">LE13FertHighIrrigOnCvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1996EarlyCvBuster</t>
+    <t xml:space="preserve">LE14CvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1996EarlyCvQL41xQL36</t>
+    <t xml:space="preserve">LE14CvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1996EarlyCvM351</t>
+    <t xml:space="preserve">LE14CvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1996LateCvBuster</t>
+    <t xml:space="preserve">LE15CvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1996LateCvQL41xQL36</t>
+    <t xml:space="preserve">LE15CvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1996LateCvM351</t>
+    <t xml:space="preserve">LE15CvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1997LateCvBuster</t>
+    <t xml:space="preserve">LE17CvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1997LateCvCSH13R</t>
+    <t xml:space="preserve">LE17CvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1997LateCvM351</t>
+    <t xml:space="preserve">LE17CvM351</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertMedCvBuster</t>
+    <t xml:space="preserve">LE19FertMedCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertLowCvCSH13R</t>
+    <t xml:space="preserve">LE19FertLowCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertOffCvBuster</t>
+    <t xml:space="preserve">LE19FertOffCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertLowCvBuster</t>
+    <t xml:space="preserve">LE19FertLowCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertHighCvBuster</t>
+    <t xml:space="preserve">LE19FertHighCvBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertOffCvCSH13R</t>
+    <t xml:space="preserve">LE19FertOffCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertMedCvCSH13R</t>
+    <t xml:space="preserve">LE19FertMedCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1998FertHighCvCSH13R</t>
+    <t xml:space="preserve">LE19FertHighCvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvA35xQL36FertLow</t>
+    <t xml:space="preserve">LE21CvA35xQL36FertLow</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvA35xQL36FertHigh</t>
+    <t xml:space="preserve">LE21CvA35xQL36FertHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvCSH13RFertLow</t>
+    <t xml:space="preserve">LE21CvCSH13RFertLow</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvQL39xQL36FertLow</t>
+    <t xml:space="preserve">LE21CvQL39xQL36FertLow</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvCSH13RFertMed</t>
+    <t xml:space="preserve">LE21CvCSH13RFertMed</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvA35xQL36FertMed</t>
+    <t xml:space="preserve">LE21CvA35xQL36FertMed</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvQL39xQL36FertMed</t>
+    <t xml:space="preserve">LE21CvQL39xQL36FertMed</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvQL39xQL36FertHigh</t>
+    <t xml:space="preserve">LE21CvQL39xQL36FertHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">Lawes1999CvCSH13RFertHigh</t>
+    <t xml:space="preserve">LE21CvCSH13RFertHigh</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:BE2195"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1812" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1820" activeCellId="32" sqref="B1899 B1910 B1919 B1928 B1935 B1939 B1941 B1950 B1959 B1973 B1982 B1991 B1993 B1997 B2007 B2021 B2031 B2035 B2038 B2050 B2065 B2078 B2095 B2105 B2114 B2123 B2132 B2141 B2143 B2152 B2154 B2171 C1820"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A955" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B982" activeCellId="1" sqref="B1890:B2195 B982"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -972,7 +972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>35373</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>6.889</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>35373</v>
       </c>

</xml_diff>

<commit_message>
Change sorghum hermitage simulations to 8 experiments
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -268,76 +268,76 @@
     <t xml:space="preserve">BW8CvQL41xQL36FertLowIrrigOff</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertHighIrrigOnCvBuster</t>
+    <t xml:space="preserve">HE1CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertHighIrrigOnCvQL41xQL36</t>
+    <t xml:space="preserve">HE1CultivarQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertHighIrrigOnCvM351</t>
+    <t xml:space="preserve">HE1CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertLowIrrigOnCvQL41xQL36</t>
+    <t xml:space="preserve">HE2CultivarQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertLowIrrigOnCvBuster</t>
+    <t xml:space="preserve">HE2CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertLowIrrigOnCvM351</t>
+    <t xml:space="preserve">HE2CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertHighIrrigOffCvQL41xQL36</t>
+    <t xml:space="preserve">HE3CultivarQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertHighIrrigOffCvBuster</t>
+    <t xml:space="preserve">HE3CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertHighIrrigOffCvM351</t>
+    <t xml:space="preserve">HE3CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertLowIrrigOffCvQL41xQL36</t>
+    <t xml:space="preserve">HE4CultivarQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertLowIrrigOffCvBuster</t>
+    <t xml:space="preserve">HE4CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE1-4FertLowIrrigOffCvM351</t>
+    <t xml:space="preserve">HE4CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertHighIrrigHighCvBuster</t>
+    <t xml:space="preserve">HE5CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertHighIrrigHighCvM351</t>
+    <t xml:space="preserve">HE5CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertHighIrrigHighCvCSH13R</t>
+    <t xml:space="preserve">HE5CultivarCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertLowIrrigHighCvBuster</t>
+    <t xml:space="preserve">HE6CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertLowIrrigHighCvM351</t>
+    <t xml:space="preserve">HE6CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertLowIrrigHighCvCSH13R</t>
+    <t xml:space="preserve">HE6CultivarCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertHighIrrigLowCvBuster</t>
+    <t xml:space="preserve">HE7CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertHighIrrigLowCvM351</t>
+    <t xml:space="preserve">HE7CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertHighIrrigLowCvCSH13R</t>
+    <t xml:space="preserve">HE7CultivarCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertLowIrrigLowCvBuster</t>
+    <t xml:space="preserve">HE8CultivarBuster</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertLowIrrigLowCvM351</t>
+    <t xml:space="preserve">HE8CultivarM35-1</t>
   </si>
   <si>
-    <t xml:space="preserve">HE5-8FertLowIrrigLowCvCSH13R</t>
+    <t xml:space="preserve">HE8CultivarCSH13R</t>
   </si>
   <si>
     <t xml:space="preserve">LE13FertLowirrigOffCvBuster</t>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:BE2195"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A955" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B982" activeCellId="1" sqref="B1890:B2195 B982"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A877" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B900" activeCellId="24" sqref="B1269 B1271 B1274 B1277 B1280 B1283 B1286:B1287 B1292 B1295 B1302 B1308 B1312 B1316 B1319:B1320 B1323 B1325 B1328 B1332 B1336 B1338 B1340 B1343 B1345 B1347 B900"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed simulation names in sorghum observed data
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
+++ b/Tests/UnderReview/Sorghum/obs/DailyObserved.xlsx
@@ -364,7 +364,7 @@
     <t xml:space="preserve">LE14CvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">LE14CvM351</t>
+    <t xml:space="preserve">LE14CvM35-1</t>
   </si>
   <si>
     <t xml:space="preserve">LE15CvBuster</t>
@@ -373,7 +373,7 @@
     <t xml:space="preserve">LE15CvQL41xQL36</t>
   </si>
   <si>
-    <t xml:space="preserve">LE15CvM351</t>
+    <t xml:space="preserve">LE15CvM35-1</t>
   </si>
   <si>
     <t xml:space="preserve">LE17CvBuster</t>
@@ -382,7 +382,7 @@
     <t xml:space="preserve">LE17CvCSH13R</t>
   </si>
   <si>
-    <t xml:space="preserve">LE17CvM351</t>
+    <t xml:space="preserve">LE17CvM35-1</t>
   </si>
   <si>
     <t xml:space="preserve">LE19FertMedCvBuster</t>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:BE2195"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A877" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B900" activeCellId="24" sqref="B1269 B1271 B1274 B1277 B1280 B1283 B1286:B1287 B1292 B1295 B1302 B1308 B1312 B1316 B1319:B1320 B1323 B1325 B1328 B1332 B1336 B1338 B1340 B1343 B1345 B1347 B900"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1455" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1486" activeCellId="20" sqref="B1639 B1642 B1645 B1651 B1654 B1657 B1660 B1663 B1666 B1670 B1674 B1677 B1679:B1680 B1682 B1685 B1688 B1691 B1694 B1698 B1700:B1702 I1486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>